<commit_message>
add P3388 test vector generation
</commit_message>
<xml_diff>
--- a/config_p3388/extreme_rfi.xlsx
+++ b/config_p3388/extreme_rfi.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\meas\p3388_general_rfi_tv\config_p3388\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5E91B1-D88D-479D-9BE4-CBBC6C13D6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04824762-DF9F-4424-A5F0-4596FEAC1CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6900" yWindow="1875" windowWidth="17085" windowHeight="15915" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
   </si>
 </sst>
 </file>
@@ -492,10 +495,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O184"/>
+  <dimension ref="A1:O185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P51" sqref="P51:P52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,11 +568,11 @@
         <v>0.96499999999999997</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" ref="E2:E5" si="0">1-D2</f>
+        <f t="shared" ref="E2:E6" si="0">1-D2</f>
         <v>3.5000000000000031E-2</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" ref="F2:F5" si="1">1-G2</f>
+        <f t="shared" ref="F2:F6" si="1">1-G2</f>
         <v>3.5000000000000031E-2</v>
       </c>
       <c r="G2" s="2">
@@ -608,8 +611,8 @@
         <v>10</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C4" ca="1" si="2">RANDBETWEEN(1,1024)</f>
-        <v>973</v>
+        <f ca="1">RANDBETWEEN(100,300)</f>
+        <v>234</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -627,12 +630,10 @@
         <v>11</v>
       </c>
       <c r="I3" s="2">
-        <f ca="1">RANDBETWEEN(100,200)</f>
-        <v>174</v>
+        <v>200</v>
       </c>
       <c r="J3" s="2">
-        <f ca="1">RANDBETWEEN(10,50)</f>
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>11</v>
@@ -658,8 +659,8 @@
         <v>10</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <f ca="1">RANDBETWEEN(350,650)</f>
+        <v>435</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -677,12 +678,10 @@
         <v>11</v>
       </c>
       <c r="I4" s="2">
-        <f ca="1">RANDBETWEEN(100,200)</f>
-        <v>178</v>
+        <v>200</v>
       </c>
       <c r="J4" s="2">
-        <f ca="1">RANDBETWEEN(10,50)</f>
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>11</v>
@@ -702,50 +701,43 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="1">
-        <f ca="1">RANDBETWEEN(1,1024)</f>
-        <v>1009</v>
+        <v>900</v>
       </c>
       <c r="D5" s="2">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>4.0000000000000036E-2</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
-        <v>0.44999999999999996</v>
+        <v>0</v>
       </c>
       <c r="G5" s="2">
-        <v>0.55000000000000004</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="1">
-        <f ca="1">RANDBETWEEN(1,30)</f>
-        <v>19</v>
+      <c r="I5" s="2">
+        <v>200</v>
       </c>
       <c r="J5" s="2">
-        <f ca="1">RAND()*3</f>
-        <v>1.239951761954897</v>
+        <v>50</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="1">
-        <f ca="1">RANDBETWEEN(-10,10)</f>
-        <v>7</v>
+      <c r="L5" s="2">
+        <v>0</v>
       </c>
       <c r="M5" s="2">
-        <f ca="1">RAND()*3</f>
-        <v>0.77436634931354531</v>
+        <v>6</v>
       </c>
       <c r="N5" s="1">
         <v>0</v>
@@ -756,52 +748,50 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" ref="C6:C64" ca="1" si="3">RANDBETWEEN(1,1024)</f>
-        <v>376</v>
+        <f ca="1">RANDBETWEEN(700,1000)</f>
+        <v>902</v>
       </c>
       <c r="D6" s="2">
-        <f>D5</f>
         <v>0.96</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" ref="E6:E14" si="4">1-D6</f>
+        <f t="shared" si="0"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" ref="F6:F14" si="5">1-G6</f>
+        <f t="shared" si="1"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G6" s="2">
-        <f>G5</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" ref="I6:I64" ca="1" si="6">RANDBETWEEN(1,30)</f>
-        <v>17</v>
+        <f ca="1">RANDBETWEEN(1,30)</f>
+        <v>27</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" ref="J6:J64" ca="1" si="7">RAND()*3</f>
-        <v>0.78698448768366147</v>
+        <f ca="1">RAND()*3</f>
+        <v>9.3547861164784751E-2</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" ref="L6:L64" ca="1" si="8">RANDBETWEEN(-10,10)</f>
-        <v>-2</v>
+        <f ca="1">RANDBETWEEN(-10,10)</f>
+        <v>-6</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" ref="M6:M64" ca="1" si="9">RAND()*3</f>
-        <v>2.1830833468220048</v>
+        <f ca="1">RAND()*3</f>
+        <v>0.5288422117783288</v>
       </c>
       <c r="N6" s="1">
         <v>0</v>
@@ -812,52 +802,52 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>160</v>
+        <f t="shared" ref="C7:C65" ca="1" si="2">RANDBETWEEN(1,1024)</f>
+        <v>615</v>
       </c>
       <c r="D7" s="2">
-        <f t="shared" ref="D7:D14" si="10">D6</f>
+        <f>D6</f>
         <v>0.96</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="E7:E15" si="3">1-D7</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F7:F15" si="4">1-G7</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ref="G7:G14" si="11">G6</f>
+        <f>G6</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ref="I7:I65" ca="1" si="5">RANDBETWEEN(1,30)</f>
         <v>27</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.9786968341100319</v>
+        <f t="shared" ref="J7:J65" ca="1" si="6">RAND()*3</f>
+        <v>0.30783541571481654</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-10</v>
+        <f t="shared" ref="L7:L65" ca="1" si="7">RANDBETWEEN(-10,10)</f>
+        <v>-1</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.7417520290636854</v>
+        <f t="shared" ref="M7:M65" ca="1" si="8">RAND()*3</f>
+        <v>2.9647112445021375</v>
       </c>
       <c r="N7" s="1">
         <v>0</v>
@@ -868,52 +858,52 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>681</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>722</v>
       </c>
       <c r="D8" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="D8:D15" si="9">D7</f>
         <v>0.96</v>
       </c>
       <c r="E8" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="4"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F8" s="2">
-        <f t="shared" si="5"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" ref="G8:G15" si="10">G7</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>23</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.8308435220111168</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.13576789665000266</v>
       </c>
       <c r="K8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.54437889753120661</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.14226350683834</v>
       </c>
       <c r="N8" s="1">
         <v>0</v>
@@ -924,52 +914,52 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>403</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>242</v>
       </c>
       <c r="D9" s="2">
+        <f t="shared" si="9"/>
+        <v>0.96</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="10"/>
-        <v>0.96</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" si="4"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" si="5"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G9" s="2">
-        <f t="shared" si="11"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.3052567092605987</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.21325574623609544</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-10</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.48583039693481933</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.688719181253354</v>
       </c>
       <c r="N9" s="1">
         <v>0</v>
@@ -980,52 +970,52 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>685</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>319</v>
       </c>
       <c r="D10" s="2">
+        <f t="shared" si="9"/>
+        <v>0.96</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="10"/>
-        <v>0.96</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="4"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F10" s="2">
-        <f t="shared" si="5"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G10" s="2">
-        <f t="shared" si="11"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>11</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>29</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.6584021734376058</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>8.562082947990679E-2</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-6</v>
       </c>
       <c r="M10" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.40286560498279922</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.28376478723763443</v>
       </c>
       <c r="N10" s="1">
         <v>0</v>
@@ -1036,52 +1026,52 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>411</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>26</v>
       </c>
       <c r="D11" s="2">
+        <f t="shared" si="9"/>
+        <v>0.96</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="10"/>
-        <v>0.96</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="4"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F11" s="2">
-        <f t="shared" si="5"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G11" s="2">
-        <f t="shared" si="11"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>18</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>29</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.3872633256099456</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.5518395570773822</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>6</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.4597592520914353</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.62489047397191511</v>
       </c>
       <c r="N11" s="1">
         <v>0</v>
@@ -1092,52 +1082,52 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1">
-        <f ca="1">RANDBETWEEN(1,1024)</f>
-        <v>957</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>23</v>
       </c>
       <c r="D12" s="2">
+        <f t="shared" si="9"/>
+        <v>0.96</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G12" s="2">
         <f t="shared" si="10"/>
-        <v>0.96</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="4"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="5"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G12" s="2">
-        <f t="shared" si="11"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>11</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.69672118635591085</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.1053929342855455</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L12" s="1">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>0</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.63202938294216338</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.89063974597926832</v>
       </c>
       <c r="N12" s="1">
         <v>0</v>
@@ -1148,52 +1138,52 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>689</v>
+        <f ca="1">RANDBETWEEN(1,1024)</f>
+        <v>532</v>
       </c>
       <c r="D13" s="2">
+        <f t="shared" si="9"/>
+        <v>0.96</v>
+      </c>
+      <c r="E13" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G13" s="2">
         <f t="shared" si="10"/>
-        <v>0.96</v>
-      </c>
-      <c r="E13" s="2">
-        <f t="shared" si="4"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F13" s="2">
-        <f t="shared" si="5"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G13" s="2">
-        <f t="shared" si="11"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>22</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.9583503414886478</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.549603955492171</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L13" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>8</v>
       </c>
       <c r="M13" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.94037461454393578</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.98060021162222799</v>
       </c>
       <c r="N13" s="1">
         <v>0</v>
@@ -1204,52 +1194,52 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1016</v>
       </c>
       <c r="D14" s="2">
+        <f t="shared" si="9"/>
+        <v>0.96</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" si="3"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="4"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G14" s="2">
         <f t="shared" si="10"/>
-        <v>0.96</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" si="4"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F14" s="2">
-        <f t="shared" si="5"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G14" s="2">
-        <f t="shared" si="11"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.4804074286368945</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.7610895711018115</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-3</v>
       </c>
       <c r="M14" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.87848595288450138</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.6094969793550709</v>
       </c>
       <c r="N14" s="1">
         <v>0</v>
@@ -1260,52 +1250,52 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>471</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>816</v>
       </c>
       <c r="D15" s="2">
-        <f t="shared" ref="D15:D22" si="12">D14</f>
+        <f t="shared" si="9"/>
         <v>0.96</v>
       </c>
       <c r="E15" s="2">
-        <f t="shared" ref="E15:E22" si="13">1-D15</f>
+        <f t="shared" si="3"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F15" s="2">
-        <f t="shared" ref="F15:F22" si="14">1-G15</f>
+        <f t="shared" si="4"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G15" s="2">
-        <f t="shared" ref="G15:G22" si="15">G14</f>
+        <f t="shared" si="10"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>18</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>2</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.1111843487621922</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.2318096110500325</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L15" s="1">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>5</v>
       </c>
       <c r="M15" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.9461120241462795</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.1777803695513391</v>
       </c>
       <c r="N15" s="1">
         <v>0</v>
@@ -1316,52 +1306,52 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>732</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>173</v>
       </c>
       <c r="D16" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="D16:D23" si="11">D15</f>
         <v>0.96</v>
       </c>
       <c r="E16" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" ref="E16:E23" si="12">1-D16</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F16" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="F16:F23" si="13">1-G16</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="G16" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="G16:G23" si="14">G15</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="J16" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.9170837537386993</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L16" s="1">
+        <f t="shared" ca="1" si="7"/>
         <v>4</v>
       </c>
-      <c r="J16" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.5676921952323228</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L16" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-10</v>
-      </c>
       <c r="M16" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.88207881517223075</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.5491401334396575</v>
       </c>
       <c r="N16" s="1">
         <v>0</v>
@@ -1372,52 +1362,52 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>538</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1020</v>
       </c>
       <c r="D17" s="2">
+        <f t="shared" si="11"/>
+        <v>0.96</v>
+      </c>
+      <c r="E17" s="2">
         <f t="shared" si="12"/>
-        <v>0.96</v>
-      </c>
-      <c r="E17" s="2">
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F17" s="2">
         <f t="shared" si="13"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F17" s="2">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G17" s="2">
         <f t="shared" si="14"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G17" s="2">
-        <f t="shared" si="15"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.2068237793393148</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.2367633474839295</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L17" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
       </c>
       <c r="M17" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.5251854745969147</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.4101805265994907</v>
       </c>
       <c r="N17" s="1">
         <v>0</v>
@@ -1428,52 +1418,52 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>675</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>127</v>
       </c>
       <c r="D18" s="2">
+        <f t="shared" si="11"/>
+        <v>0.96</v>
+      </c>
+      <c r="E18" s="2">
         <f t="shared" si="12"/>
-        <v>0.96</v>
-      </c>
-      <c r="E18" s="2">
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F18" s="2">
         <f t="shared" si="13"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F18" s="2">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G18" s="2">
         <f t="shared" si="14"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G18" s="2">
-        <f t="shared" si="15"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>30</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.19985581339570713</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.0346218255291917</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M18" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.62395927543036</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.6319931387912034</v>
       </c>
       <c r="N18" s="1">
         <v>0</v>
@@ -1484,52 +1474,52 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>796</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>517</v>
       </c>
       <c r="D19" s="2">
+        <f t="shared" si="11"/>
+        <v>0.96</v>
+      </c>
+      <c r="E19" s="2">
         <f t="shared" si="12"/>
-        <v>0.96</v>
-      </c>
-      <c r="E19" s="2">
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F19" s="2">
         <f t="shared" si="13"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F19" s="2">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G19" s="2">
         <f t="shared" si="14"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G19" s="2">
-        <f t="shared" si="15"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>24</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>15</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.37673241732246054</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.6298564374124007</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L19" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-5</v>
       </c>
       <c r="M19" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>9.8989090656740997E-2</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.81286113163423312</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
@@ -1540,52 +1530,52 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>520</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>53</v>
       </c>
       <c r="D20" s="2">
+        <f t="shared" si="11"/>
+        <v>0.96</v>
+      </c>
+      <c r="E20" s="2">
         <f t="shared" si="12"/>
-        <v>0.96</v>
-      </c>
-      <c r="E20" s="2">
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F20" s="2">
         <f t="shared" si="13"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F20" s="2">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G20" s="2">
         <f t="shared" si="14"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G20" s="2">
-        <f t="shared" si="15"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="J20" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>1.846543481262676</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20" s="1">
+        <f t="shared" ca="1" si="7"/>
         <v>2</v>
       </c>
-      <c r="J20" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.28714347331843115</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L20" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-1</v>
-      </c>
       <c r="M20" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.2523959172435482</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.738178110672405</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -1596,52 +1586,52 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>744</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>285</v>
       </c>
       <c r="D21" s="2">
+        <f t="shared" si="11"/>
+        <v>0.96</v>
+      </c>
+      <c r="E21" s="2">
         <f t="shared" si="12"/>
-        <v>0.96</v>
-      </c>
-      <c r="E21" s="2">
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F21" s="2">
         <f t="shared" si="13"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F21" s="2">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G21" s="2">
         <f t="shared" si="14"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G21" s="2">
-        <f t="shared" si="15"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>19</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.9641436599226626</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.3206181118339371</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L21" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>6</v>
       </c>
       <c r="M21" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.499903855641878</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.3242474568588607</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
@@ -1652,52 +1642,52 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>859</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>754</v>
       </c>
       <c r="D22" s="2">
+        <f t="shared" si="11"/>
+        <v>0.96</v>
+      </c>
+      <c r="E22" s="2">
         <f t="shared" si="12"/>
-        <v>0.96</v>
-      </c>
-      <c r="E22" s="2">
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F22" s="2">
         <f t="shared" si="13"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F22" s="2">
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G22" s="2">
         <f t="shared" si="14"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="G22" s="2">
-        <f t="shared" si="15"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>20</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>17</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.75329973583529319</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.8836395630770952</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L22" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-1</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>6</v>
       </c>
       <c r="M22" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.5626066414159618</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.4656796472161213</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
@@ -1708,52 +1698,52 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C23" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>923</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>708</v>
       </c>
       <c r="D23" s="2">
-        <f t="shared" ref="D23:D64" si="16">D22</f>
+        <f t="shared" si="11"/>
         <v>0.96</v>
       </c>
       <c r="E23" s="2">
-        <f t="shared" ref="E23:E24" si="17">1-D23</f>
+        <f t="shared" si="12"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F23" s="2">
-        <f t="shared" ref="F23:F24" si="18">1-G23</f>
+        <f t="shared" si="13"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G23" s="2">
-        <f t="shared" ref="G23:G64" si="19">G22</f>
+        <f t="shared" si="14"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="J23" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.400016158712579</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" ca="1" si="7"/>
         <v>5</v>
       </c>
-      <c r="J23" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.7105296716069618</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L23" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>8</v>
-      </c>
       <c r="M23" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.5445062285839115</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.3057131893121872</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
@@ -1764,52 +1754,52 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>897</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>640</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="D24:D65" si="15">D23</f>
         <v>0.96</v>
       </c>
       <c r="E24" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="E24:E25" si="16">1-D24</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F24" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" ref="F24:F25" si="17">1-G24</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="G24" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" ref="G24:G65" si="18">G23</f>
         <v>0.55000000000000004</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>28</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.9371428207401431</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.6966422263077816</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M24" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.2378866581422616</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.7784713071425764</v>
       </c>
       <c r="N24" s="1">
         <v>0</v>
@@ -1826,46 +1816,46 @@
         <v>10</v>
       </c>
       <c r="C25" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>899</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>667</v>
       </c>
       <c r="D25" s="2">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+      <c r="E25" s="2">
         <f t="shared" si="16"/>
-        <v>0.96</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" ref="E25:E34" si="20">1-D25</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F25" s="2">
-        <f t="shared" ref="F25:F34" si="21">1-G25</f>
+        <f t="shared" si="17"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G25" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>16</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>26</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>8.6679666140593525E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.9672634417980621</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L25" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>3</v>
       </c>
       <c r="M25" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.0042233987197835</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.81381896406728316</v>
       </c>
       <c r="N25" s="1">
         <v>0</v>
@@ -1882,46 +1872,46 @@
         <v>10</v>
       </c>
       <c r="C26" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>676</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>283</v>
       </c>
       <c r="D26" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E26" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="E26:E35" si="19">1-D26</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F26" s="2">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="F26:F35" si="20">1-G26</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="G26" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>23</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.97462552592879992</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.49479197523072238</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L26" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M26" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.8256630139080423</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.3061086041620336</v>
       </c>
       <c r="N26" s="1">
         <v>0</v>
@@ -1938,46 +1928,46 @@
         <v>10</v>
       </c>
       <c r="C27" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>375</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>987</v>
       </c>
       <c r="D27" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E27" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F27" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F27" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G27" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>22</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.2922770450740333</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.2489275608330632</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L27" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
       </c>
       <c r="M27" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.91834589072161688</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.6939629006545482</v>
       </c>
       <c r="N27" s="1">
         <v>0</v>
@@ -1994,46 +1984,46 @@
         <v>10</v>
       </c>
       <c r="C28" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>136</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>605</v>
       </c>
       <c r="D28" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E28" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F28" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G28" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>16</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.1549199623276589</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.9126880710932088</v>
       </c>
       <c r="K28" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M28" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.0047985382316567</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.90422280815668232</v>
       </c>
       <c r="N28" s="1">
         <v>0</v>
@@ -2050,46 +2040,46 @@
         <v>10</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>543</v>
       </c>
       <c r="D29" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E29" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F29" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G29" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.1438259982009704</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.1267646258343764</v>
       </c>
       <c r="K29" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L29" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-9</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M29" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.39457754430430125</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.4483397749031135</v>
       </c>
       <c r="N29" s="1">
         <v>0</v>
@@ -2106,46 +2096,46 @@
         <v>10</v>
       </c>
       <c r="C30" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>467</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>606</v>
       </c>
       <c r="D30" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E30" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F30" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F30" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G30" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>29</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>22</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.6979224057852291</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.3062325599345053</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L30" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-3</v>
       </c>
       <c r="M30" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.88125641702301083</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.6962240824930106</v>
       </c>
       <c r="N30" s="1">
         <v>0</v>
@@ -2162,46 +2152,46 @@
         <v>10</v>
       </c>
       <c r="C31" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>587</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>555</v>
       </c>
       <c r="D31" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E31" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F31" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F31" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G31" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>25</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.2698467462594654</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.4113038875923245</v>
       </c>
       <c r="K31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L31" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>5</v>
       </c>
       <c r="M31" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.7649481783013212</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.4101323673169792</v>
       </c>
       <c r="N31" s="1">
         <v>0</v>
@@ -2218,46 +2208,46 @@
         <v>10</v>
       </c>
       <c r="C32" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>950</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>772</v>
       </c>
       <c r="D32" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E32" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F32" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F32" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G32" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>20</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.2123208142421003</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.50715478381957557</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L32" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>8</v>
       </c>
       <c r="M32" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.0677073278031224</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.9222183822869188</v>
       </c>
       <c r="N32" s="1">
         <v>0</v>
@@ -2274,46 +2264,46 @@
         <v>10</v>
       </c>
       <c r="C33" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>580</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>127</v>
       </c>
       <c r="D33" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E33" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F33" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F33" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G33" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>14</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.5893300602574494</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.64441015738039842</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L33" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
       </c>
       <c r="M33" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.1010602384353017</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.112220500811171</v>
       </c>
       <c r="N33" s="1">
         <v>0</v>
@@ -2330,46 +2320,46 @@
         <v>10</v>
       </c>
       <c r="C34" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>624</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>333</v>
       </c>
       <c r="D34" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E34" s="2">
+        <f t="shared" si="19"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F34" s="2">
         <f t="shared" si="20"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" si="21"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G34" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>9</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.0879347103422994</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6.4654068941974563E-2</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
       </c>
       <c r="M34" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.9929861298027105</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.6098474349167855</v>
       </c>
       <c r="N34" s="1">
         <v>0</v>
@@ -2386,46 +2376,46 @@
         <v>10</v>
       </c>
       <c r="C35" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>616</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>959</v>
       </c>
       <c r="D35" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E35" s="2">
-        <f t="shared" ref="E35:E64" si="22">1-D35</f>
+        <f t="shared" si="19"/>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F35" s="2">
-        <f t="shared" ref="F35:F64" si="23">1-G35</f>
+        <f t="shared" si="20"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G35" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.56071971474028348</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.38600439502360218</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L35" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-5</v>
       </c>
       <c r="M35" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.463341126923301</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.56734317633626308</v>
       </c>
       <c r="N35" s="1">
         <v>0</v>
@@ -2442,46 +2432,46 @@
         <v>10</v>
       </c>
       <c r="C36" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>874</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>690</v>
       </c>
       <c r="D36" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E36" s="2">
-        <f t="shared" si="22"/>
+        <f t="shared" ref="E36:E65" si="21">1-D36</f>
         <v>4.0000000000000036E-2</v>
       </c>
       <c r="F36" s="2">
-        <f t="shared" si="23"/>
+        <f t="shared" ref="F36:F65" si="22">1-G36</f>
         <v>0.44999999999999996</v>
       </c>
       <c r="G36" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>24</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.8713513401971076</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.6233809312539955</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L36" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-5</v>
       </c>
       <c r="M36" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.71712371284209087</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.7702962967496152</v>
       </c>
       <c r="N36" s="1">
         <v>0</v>
@@ -2498,46 +2488,46 @@
         <v>10</v>
       </c>
       <c r="C37" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>315</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>756</v>
       </c>
       <c r="D37" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E37" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F37" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F37" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G37" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>18</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.99364338820867837</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.7017674914022813</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L37" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-9</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
       </c>
       <c r="M37" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.0912500794560329</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.5825351411892035</v>
       </c>
       <c r="N37" s="1">
         <v>0</v>
@@ -2554,46 +2544,46 @@
         <v>10</v>
       </c>
       <c r="C38" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>51</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>598</v>
       </c>
       <c r="D38" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E38" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F38" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F38" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G38" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>15</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>23</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.7234078929671326</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.9514941631405458</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L38" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>8</v>
       </c>
       <c r="M38" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.16618648647451306</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.6693806736535124</v>
       </c>
       <c r="N38" s="1">
         <v>0</v>
@@ -2610,46 +2600,46 @@
         <v>10</v>
       </c>
       <c r="C39" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>349</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>379</v>
       </c>
       <c r="D39" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E39" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F39" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F39" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G39" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>22</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.94004500118226064</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.63054838072040675</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L39" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>9</v>
       </c>
       <c r="M39" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.7636952777603403</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.16799040282708944</v>
       </c>
       <c r="N39" s="1">
         <v>0</v>
@@ -2666,46 +2656,46 @@
         <v>10</v>
       </c>
       <c r="C40" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>156</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>686</v>
       </c>
       <c r="D40" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E40" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F40" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F40" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G40" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>30</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>13</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.3854376643864827</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.6012874329221134</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L40" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-10</v>
       </c>
       <c r="M40" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.0202776881081181</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.834602752577855</v>
       </c>
       <c r="N40" s="1">
         <v>0</v>
@@ -2722,46 +2712,46 @@
         <v>10</v>
       </c>
       <c r="C41" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>937</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>280</v>
       </c>
       <c r="D41" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E41" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F41" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F41" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G41" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>20</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.8619995108010654</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.178359267678619</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L41" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-9</v>
       </c>
       <c r="M41" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.2713814269959125</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.2196115178453839</v>
       </c>
       <c r="N41" s="1">
         <v>0</v>
@@ -2778,46 +2768,46 @@
         <v>10</v>
       </c>
       <c r="C42" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>718</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>165</v>
       </c>
       <c r="D42" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E42" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F42" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F42" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G42" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>1</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.2176614560282619</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>8.003979040643161E-2</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L42" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-10</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
       </c>
       <c r="M42" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.5350420828151314</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.91011233084580212</v>
       </c>
       <c r="N42" s="1">
         <v>0</v>
@@ -2834,46 +2824,46 @@
         <v>10</v>
       </c>
       <c r="C43" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>914</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>909</v>
       </c>
       <c r="D43" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E43" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F43" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F43" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G43" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.7029628960792116</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.5020654249149352</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L43" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>4</v>
       </c>
       <c r="M43" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.5886615687051728</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.4412773335023716</v>
       </c>
       <c r="N43" s="1">
         <v>0</v>
@@ -2890,46 +2880,46 @@
         <v>10</v>
       </c>
       <c r="C44" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>601</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
       <c r="D44" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E44" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F44" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F44" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G44" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.61112223351090533</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.15693528967745629</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L44" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-10</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>10</v>
       </c>
       <c r="M44" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.4150073026526673</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.0904242593226763</v>
       </c>
       <c r="N44" s="1">
         <v>0</v>
@@ -2946,46 +2936,46 @@
         <v>10</v>
       </c>
       <c r="C45" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>77</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>790</v>
       </c>
       <c r="D45" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E45" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F45" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F45" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G45" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>7</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.3339974366809155</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.96024920398858304</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L45" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M45" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.3342699276598546</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.9729772227603406</v>
       </c>
       <c r="N45" s="1">
         <v>0</v>
@@ -3002,46 +2992,46 @@
         <v>10</v>
       </c>
       <c r="C46" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>522</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>847</v>
       </c>
       <c r="D46" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E46" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F46" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F46" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G46" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>22</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.20405656754833934</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>7.0584789393030256E-2</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L46" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>10</v>
       </c>
       <c r="M46" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.8323041270339804</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.4068929705886193</v>
       </c>
       <c r="N46" s="1">
         <v>0</v>
@@ -3058,46 +3048,46 @@
         <v>10</v>
       </c>
       <c r="C47" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>192</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>521</v>
       </c>
       <c r="D47" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E47" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F47" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F47" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G47" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>18</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>25</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.2223561905853142</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.8567792349932306</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L47" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
       </c>
       <c r="M47" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.639633143785225</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.9784729849772802</v>
       </c>
       <c r="N47" s="1">
         <v>0</v>
@@ -3114,46 +3104,46 @@
         <v>10</v>
       </c>
       <c r="C48" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>707</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>538</v>
       </c>
       <c r="D48" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E48" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F48" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F48" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G48" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>27</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>11</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.8057843609888882</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.9945652778527787</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L48" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>9</v>
       </c>
       <c r="M48" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.0675750512578546</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.17851561479748534</v>
       </c>
       <c r="N48" s="1">
         <v>0</v>
@@ -3170,46 +3160,46 @@
         <v>10</v>
       </c>
       <c r="C49" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>812</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>151</v>
       </c>
       <c r="D49" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E49" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F49" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F49" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G49" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>22</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.62531000383748048</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>6.1377762024290683E-2</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L49" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-7</v>
       </c>
       <c r="M49" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.0345937509594973</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>8.4174353510624855E-2</v>
       </c>
       <c r="N49" s="1">
         <v>0</v>
@@ -3226,46 +3216,46 @@
         <v>10</v>
       </c>
       <c r="C50" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>364</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>178</v>
       </c>
       <c r="D50" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E50" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F50" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F50" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G50" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>27</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>15</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.4355833091701076E-2</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.7931834445341628</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L50" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>7</v>
       </c>
       <c r="M50" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.5800669988462186</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.289191371248176</v>
       </c>
       <c r="N50" s="1">
         <v>0</v>
@@ -3282,46 +3272,46 @@
         <v>10</v>
       </c>
       <c r="C51" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>944</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>328</v>
       </c>
       <c r="D51" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E51" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F51" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F51" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G51" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>28</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.5103839957326866</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.6982838488155405</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L51" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
       </c>
       <c r="M51" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.986315738585287</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.485266341807908</v>
       </c>
       <c r="N51" s="1">
         <v>0</v>
@@ -3338,46 +3328,46 @@
         <v>10</v>
       </c>
       <c r="C52" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>46</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>605</v>
       </c>
       <c r="D52" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E52" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F52" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F52" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G52" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.2136774890333353</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.91838984629124432</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L52" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-10</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-2</v>
       </c>
       <c r="M52" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.9494590626188306</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.1071715802721136</v>
       </c>
       <c r="N52" s="1">
         <v>0</v>
@@ -3394,46 +3384,46 @@
         <v>10</v>
       </c>
       <c r="C53" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>945</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>961</v>
       </c>
       <c r="D53" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E53" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F53" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F53" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G53" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>26</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>8</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.4857690029973178</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.4591724998163329</v>
       </c>
       <c r="K53" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L53" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-8</v>
       </c>
       <c r="M53" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.57953513466699225</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.8666011063322916</v>
       </c>
       <c r="N53" s="1">
         <v>0</v>
@@ -3450,46 +3440,46 @@
         <v>10</v>
       </c>
       <c r="C54" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>917</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>142</v>
       </c>
       <c r="D54" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E54" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F54" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F54" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G54" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>3</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>0.41277793500730153</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.8933424302923614</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L54" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-8</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-1</v>
       </c>
       <c r="M54" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.21301988390662241</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.4427127432483289</v>
       </c>
       <c r="N54" s="1">
         <v>0</v>
@@ -3506,46 +3496,46 @@
         <v>10</v>
       </c>
       <c r="C55" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>173</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>325</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E55" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F55" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F55" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G55" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I55" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>15</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.5021626139731037</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.7978142810008564</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L55" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>1</v>
       </c>
       <c r="M55" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.2809801968940087</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.23656179636428631</v>
       </c>
       <c r="N55" s="1">
         <v>0</v>
@@ -3562,46 +3552,46 @@
         <v>10</v>
       </c>
       <c r="C56" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>59</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>72</v>
       </c>
       <c r="D56" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E56" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F56" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F56" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G56" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I56" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>28</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>26</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.3691895454181324</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.2718747482513466</v>
       </c>
       <c r="K56" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L56" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>0</v>
       </c>
       <c r="M56" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.40328076658858003</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.3655741656770026</v>
       </c>
       <c r="N56" s="1">
         <v>0</v>
@@ -3618,46 +3608,46 @@
         <v>10</v>
       </c>
       <c r="C57" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>65</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>66</v>
       </c>
       <c r="D57" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E57" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F57" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F57" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G57" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I57" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>12</v>
       </c>
       <c r="J57" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.8354136211269507</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.87545427100609763</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L57" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-1</v>
       </c>
       <c r="M57" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.7836307905118129</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>2.1039683923263093</v>
       </c>
       <c r="N57" s="1">
         <v>0</v>
@@ -3674,46 +3664,46 @@
         <v>10</v>
       </c>
       <c r="C58" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>192</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>951</v>
       </c>
       <c r="D58" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E58" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F58" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F58" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G58" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I58" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>10</v>
       </c>
       <c r="J58" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.0861466369576953</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.13772107516780274</v>
       </c>
       <c r="K58" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L58" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-3</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>9</v>
       </c>
       <c r="M58" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.9192360390338155</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.97972240582544035</v>
       </c>
       <c r="N58" s="1">
         <v>0</v>
@@ -3730,46 +3720,46 @@
         <v>10</v>
       </c>
       <c r="C59" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>605</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>41</v>
       </c>
       <c r="D59" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E59" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F59" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F59" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G59" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" ca="1" si="6"/>
+        <f t="shared" ca="1" si="5"/>
         <v>4</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.1305823166623485</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.28153188909016147</v>
       </c>
       <c r="K59" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L59" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-7</v>
       </c>
       <c r="M59" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.2889478534046335</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>1.4313961594546485</v>
       </c>
       <c r="N59" s="1">
         <v>0</v>
@@ -3786,46 +3776,46 @@
         <v>10</v>
       </c>
       <c r="C60" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>483</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>858</v>
       </c>
       <c r="D60" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E60" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F60" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F60" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G60" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I60" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>23</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>24</v>
       </c>
       <c r="J60" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.8340123142876732</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>0.83873533941612666</v>
       </c>
       <c r="K60" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L60" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-7</v>
       </c>
       <c r="M60" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.12916053107556502</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.41646075744553346</v>
       </c>
       <c r="N60" s="1">
         <v>0</v>
@@ -3842,46 +3832,46 @@
         <v>10</v>
       </c>
       <c r="C61" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>220</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>253</v>
       </c>
       <c r="D61" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E61" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F61" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F61" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G61" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I61" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>10</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>30</v>
       </c>
       <c r="J61" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.2400958651016825</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.0175419740957934</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L61" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-5</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-3</v>
       </c>
       <c r="M61" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>0.40147793570138357</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.42591358638327481</v>
       </c>
       <c r="N61" s="1">
         <v>0</v>
@@ -3898,46 +3888,46 @@
         <v>10</v>
       </c>
       <c r="C62" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>35</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>163</v>
       </c>
       <c r="D62" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E62" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F62" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F62" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G62" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I62" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>21</v>
       </c>
       <c r="J62" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.3435669262865724</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.1331246628074472</v>
       </c>
       <c r="K62" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L62" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-4</v>
       </c>
       <c r="M62" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>1.8007858765795768</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.46670398068855201</v>
       </c>
       <c r="N62" s="1">
         <v>0</v>
@@ -3954,46 +3944,46 @@
         <v>10</v>
       </c>
       <c r="C63" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>1019</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>541</v>
       </c>
       <c r="D63" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E63" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F63" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F63" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G63" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I63" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>29</v>
       </c>
       <c r="J63" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>1.1772425929484378</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>1.6881747151779503</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L63" s="1">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" ca="1" si="7"/>
         <v>10</v>
       </c>
       <c r="M63" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.1614388771925612</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.74879368717148354</v>
       </c>
       <c r="N63" s="1">
         <v>0</v>
@@ -4010,46 +4000,46 @@
         <v>10</v>
       </c>
       <c r="C64" s="1">
-        <f t="shared" ca="1" si="3"/>
-        <v>346</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>121</v>
       </c>
       <c r="D64" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>0.96</v>
       </c>
       <c r="E64" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F64" s="2">
         <f t="shared" si="22"/>
-        <v>4.0000000000000036E-2</v>
-      </c>
-      <c r="F64" s="2">
-        <f t="shared" si="23"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="G64" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.55000000000000004</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I64" s="1">
-        <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>16</v>
       </c>
       <c r="J64" s="2">
-        <f t="shared" ca="1" si="7"/>
-        <v>2.7527896553833209</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>2.4309269253963377</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>11</v>
       </c>
       <c r="L64" s="1">
-        <f t="shared" ca="1" si="8"/>
-        <v>-2</v>
+        <f t="shared" ca="1" si="7"/>
+        <v>-8</v>
       </c>
       <c r="M64" s="2">
-        <f t="shared" ca="1" si="9"/>
-        <v>2.2608974705616203</v>
+        <f t="shared" ca="1" si="8"/>
+        <v>0.89268648667537698</v>
       </c>
       <c r="N64" s="1">
         <v>0</v>
@@ -4058,15 +4048,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D65" s="2"/>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="M65" s="2"/>
-    </row>
-    <row r="66" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" s="1">
+        <f t="shared" ca="1" si="2"/>
+        <v>549</v>
+      </c>
+      <c r="D65" s="2">
+        <f t="shared" si="15"/>
+        <v>0.96</v>
+      </c>
+      <c r="E65" s="2">
+        <f t="shared" si="21"/>
+        <v>4.0000000000000036E-2</v>
+      </c>
+      <c r="F65" s="2">
+        <f t="shared" si="22"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="G65" s="2">
+        <f t="shared" si="18"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I65" s="1">
+        <f t="shared" ca="1" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="J65" s="2">
+        <f t="shared" ca="1" si="6"/>
+        <v>2.7140057290758817</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L65" s="1">
+        <f t="shared" ca="1" si="7"/>
+        <v>2</v>
+      </c>
+      <c r="M65" s="2">
+        <f t="shared" ca="1" si="8"/>
+        <v>2.8647843798512982</v>
+      </c>
+      <c r="N65" s="1">
+        <v>0</v>
+      </c>
+      <c r="O65" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
@@ -4074,7 +4112,7 @@
       <c r="J66" s="2"/>
       <c r="M66" s="2"/>
     </row>
-    <row r="67" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
@@ -4082,7 +4120,7 @@
       <c r="J67" s="2"/>
       <c r="M67" s="2"/>
     </row>
-    <row r="68" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
       <c r="F68" s="2"/>
@@ -4090,7 +4128,7 @@
       <c r="J68" s="2"/>
       <c r="M68" s="2"/>
     </row>
-    <row r="69" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
       <c r="F69" s="2"/>
@@ -4098,7 +4136,7 @@
       <c r="J69" s="2"/>
       <c r="M69" s="2"/>
     </row>
-    <row r="70" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
       <c r="F70" s="2"/>
@@ -4106,7 +4144,7 @@
       <c r="J70" s="2"/>
       <c r="M70" s="2"/>
     </row>
-    <row r="71" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
       <c r="F71" s="2"/>
@@ -4114,7 +4152,7 @@
       <c r="J71" s="2"/>
       <c r="M71" s="2"/>
     </row>
-    <row r="72" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
@@ -4122,7 +4160,7 @@
       <c r="J72" s="2"/>
       <c r="M72" s="2"/>
     </row>
-    <row r="73" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
@@ -4130,7 +4168,7 @@
       <c r="J73" s="2"/>
       <c r="M73" s="2"/>
     </row>
-    <row r="74" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
@@ -4138,7 +4176,7 @@
       <c r="J74" s="2"/>
       <c r="M74" s="2"/>
     </row>
-    <row r="75" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
@@ -4146,7 +4184,7 @@
       <c r="J75" s="2"/>
       <c r="M75" s="2"/>
     </row>
-    <row r="76" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
@@ -4154,7 +4192,7 @@
       <c r="J76" s="2"/>
       <c r="M76" s="2"/>
     </row>
-    <row r="77" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
       <c r="F77" s="2"/>
@@ -4162,7 +4200,7 @@
       <c r="J77" s="2"/>
       <c r="M77" s="2"/>
     </row>
-    <row r="78" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
       <c r="F78" s="2"/>
@@ -4170,7 +4208,7 @@
       <c r="J78" s="2"/>
       <c r="M78" s="2"/>
     </row>
-    <row r="79" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
       <c r="F79" s="2"/>
@@ -4178,7 +4216,7 @@
       <c r="J79" s="2"/>
       <c r="M79" s="2"/>
     </row>
-    <row r="80" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
@@ -5018,6 +5056,14 @@
       <c r="J184" s="2"/>
       <c r="M184" s="2"/>
     </row>
+    <row r="185" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D185" s="2"/>
+      <c r="E185" s="2"/>
+      <c r="F185" s="2"/>
+      <c r="G185" s="2"/>
+      <c r="J185" s="2"/>
+      <c r="M185" s="2"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>